<commit_message>
ENR for noise figure meter automation
write ENR Cal Files
loose and sloppy quick and dirty ENR Swizzler
qLoadENR to quickly load the ENR table
Veeos (open source)
General v Tools
</commit_message>
<xml_diff>
--- a/BigBookOfVariableNames.xlsx
+++ b/BigBookOfVariableNames.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sapplen\Documents\GitHub\sandbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF590FEB-18EC-497F-96E5-30C44C34D8D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A491EEA-641E-43E0-85D6-E5DF6249EB7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12615" yWindow="915" windowWidth="20340" windowHeight="9795" firstSheet="1" activeTab="1" xr2:uid="{008E5217-F733-4E47-9D1E-43FE184E83DE}"/>
+    <workbookView xWindow="6795" yWindow="855" windowWidth="15495" windowHeight="12660" firstSheet="1" activeTab="1" xr2:uid="{008E5217-F733-4E47-9D1E-43FE184E83DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>NGC_N19-6457</t>
   </si>
@@ -118,6 +118,27 @@
   </si>
   <si>
     <t>P1dB, C1 characterization, needed for interpolation (keep the power head in it's "happy range"), safety an overpower output power accedent, verify source power level setting tracks with actual power. Sanity check that source has enough dynamic range.</t>
+  </si>
+  <si>
+    <t>calibration</t>
+  </si>
+  <si>
+    <t>results</t>
+  </si>
+  <si>
+    <t>Model bands</t>
+  </si>
+  <si>
+    <t>Input Frequency, Band, temperature, timestamp, tech name, bench, calibration files used (timestamp)</t>
+  </si>
+  <si>
+    <t>frequency(input with corresponding output by step) , input network correction, output network correction, "happy range", timestamp</t>
+  </si>
+  <si>
+    <t>frequencies, powers, bands, LO's, step sizes per band,</t>
+  </si>
+  <si>
+    <t>calculate output frequency save and sort calibration table before save. Write a cal table plot function.</t>
   </si>
 </sst>
 </file>
@@ -515,10 +536,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2649951-24F5-4472-AC6F-7EC699D87016}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,87 +555,116 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>25</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>